<commit_message>
Update 2 Excel 1100
</commit_message>
<xml_diff>
--- a/Reg_MC.xlsx
+++ b/Reg_MC.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>Test1</t>
   </si>
@@ -345,10 +345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -369,6 +369,14 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1100</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>